<commit_message>
Updating Misc and Email workflows
</commit_message>
<xml_diff>
--- a/Data/Input/NotificationsRegions.xlsx
+++ b/Data/Input/NotificationsRegions.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SYS-QAUPBOT2\.nuget\packages\scenario4and6.performer\3.5.1\lib\net45\Data\Input\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB3D81F-305B-407A-AF6A-754FB494A488}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{216F015C-57D9-4F76-A3C6-4581D888859D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="26010" windowHeight="20160" xr2:uid="{237FB236-979A-4340-8AAB-92FBF32537FD}"/>
+    <workbookView xWindow="26160" yWindow="4770" windowWidth="16755" windowHeight="10650" xr2:uid="{237FB236-979A-4340-8AAB-92FBF32537FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Regions" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15">
   <si>
     <t>France &amp; Benelux</t>
   </si>
@@ -457,10 +457,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D8221732-6468-4127-B4C8-44062AC1A822}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+      <selection activeCell="A11" sqref="A11:XFD14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -577,11 +577,6 @@
         <v>13</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B12" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>